<commit_message>
initial commits to bring in Canadian sites
</commit_message>
<xml_diff>
--- a/tbx/STswe/functions/NRCS_Sites.xlsx
+++ b/tbx/STswe/functions/NRCS_Sites.xlsx
@@ -1,26 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Raleigh\Dropbox\MATLAB\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B374EEF1-2868-48AB-94CF-0F4D4D6C547C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052DF501-83ED-4925-8CE2-DA59FF78B2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4575" yWindow="3570" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7215" yWindow="6360" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NRCS_Sites" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8367" uniqueCount="3302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8767" uniqueCount="3403">
   <si>
     <t>SCAN</t>
   </si>
@@ -9926,6 +9938,309 @@
   </si>
   <si>
     <t>Gin Flat (course)</t>
+  </si>
+  <si>
+    <t>NaN</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>Yellowhead Lake</t>
+  </si>
+  <si>
+    <t>McBride Upper</t>
+  </si>
+  <si>
+    <t>Barkerville</t>
+  </si>
+  <si>
+    <t>Hedrick Lake</t>
+  </si>
+  <si>
+    <t>Revolution Creek</t>
+  </si>
+  <si>
+    <t>Dome Mountain</t>
+  </si>
+  <si>
+    <t>Mount Wells</t>
+  </si>
+  <si>
+    <t>Tahtsa Lake</t>
+  </si>
+  <si>
+    <t>Mt. Pondosy</t>
+  </si>
+  <si>
+    <t>Mission Ridge</t>
+  </si>
+  <si>
+    <t>Boss Mountain Mine</t>
+  </si>
+  <si>
+    <t>Yanks Peak</t>
+  </si>
+  <si>
+    <t>Tenquille Lake</t>
+  </si>
+  <si>
+    <t>Wahleach Lake</t>
+  </si>
+  <si>
+    <t>Chilliwack River</t>
+  </si>
+  <si>
+    <t>Spuzzum</t>
+  </si>
+  <si>
+    <t>Mount Cook</t>
+  </si>
+  <si>
+    <t>Azure River</t>
+  </si>
+  <si>
+    <t>Kostal Lake</t>
+  </si>
+  <si>
+    <t>Park Mountain</t>
+  </si>
+  <si>
+    <t>Celista</t>
+  </si>
+  <si>
+    <t>Mount Revelstoke</t>
+  </si>
+  <si>
+    <t>Molson Creek</t>
+  </si>
+  <si>
+    <t>Barnes Creek</t>
+  </si>
+  <si>
+    <t>St. Leon Creek</t>
+  </si>
+  <si>
+    <t>Morrissey Ridge</t>
+  </si>
+  <si>
+    <t>Moyie Mountain</t>
+  </si>
+  <si>
+    <t>Floe Lake</t>
+  </si>
+  <si>
+    <t>East Creek</t>
+  </si>
+  <si>
+    <t>Redfish Creek</t>
+  </si>
+  <si>
+    <t>Grano Creek</t>
+  </si>
+  <si>
+    <t>Mission Creek</t>
+  </si>
+  <si>
+    <t>Brenda Mine</t>
+  </si>
+  <si>
+    <t>Blackwall Peak</t>
+  </si>
+  <si>
+    <t>Nostetuko River</t>
+  </si>
+  <si>
+    <t>Mosley Creek Upper</t>
+  </si>
+  <si>
+    <t>Squamish River Upper</t>
+  </si>
+  <si>
+    <t>Wolf River Upper</t>
+  </si>
+  <si>
+    <t>Jump Creek</t>
+  </si>
+  <si>
+    <t>Burnt Bridge Creek</t>
+  </si>
+  <si>
+    <t>Pine Pass</t>
+  </si>
+  <si>
+    <t>Pulpit Lake</t>
+  </si>
+  <si>
+    <t>Kwadacha North</t>
+  </si>
+  <si>
+    <t>Aiken Lake</t>
+  </si>
+  <si>
+    <t>Lu Lake</t>
+  </si>
+  <si>
+    <t>Shedin Creek</t>
+  </si>
+  <si>
+    <t>Tsai Creek</t>
+  </si>
+  <si>
+    <t>Cedar-Kiteen</t>
+  </si>
+  <si>
+    <t>Kinaskan Lake</t>
+  </si>
+  <si>
+    <t>1A01P</t>
+  </si>
+  <si>
+    <t>1A02P</t>
+  </si>
+  <si>
+    <t>1A03P</t>
+  </si>
+  <si>
+    <t>1A14P</t>
+  </si>
+  <si>
+    <t>1A17P</t>
+  </si>
+  <si>
+    <t>1A19P</t>
+  </si>
+  <si>
+    <t>1B01P</t>
+  </si>
+  <si>
+    <t>1B02P</t>
+  </si>
+  <si>
+    <t>1B08P</t>
+  </si>
+  <si>
+    <t>1C12P</t>
+  </si>
+  <si>
+    <t>1C18P</t>
+  </si>
+  <si>
+    <t>1C20P</t>
+  </si>
+  <si>
+    <t>1C41P</t>
+  </si>
+  <si>
+    <t>1D06P</t>
+  </si>
+  <si>
+    <t>1D09P</t>
+  </si>
+  <si>
+    <t>1D17P</t>
+  </si>
+  <si>
+    <t>1D19P</t>
+  </si>
+  <si>
+    <t>1E02P</t>
+  </si>
+  <si>
+    <t>1E08P</t>
+  </si>
+  <si>
+    <t>1E10P</t>
+  </si>
+  <si>
+    <t>1F03P</t>
+  </si>
+  <si>
+    <t>1F06P</t>
+  </si>
+  <si>
+    <t>2A06P</t>
+  </si>
+  <si>
+    <t>2A21P</t>
+  </si>
+  <si>
+    <t>2B06P</t>
+  </si>
+  <si>
+    <t>2B08P</t>
+  </si>
+  <si>
+    <t>2C09Q</t>
+  </si>
+  <si>
+    <t>2C10P</t>
+  </si>
+  <si>
+    <t>2C14P</t>
+  </si>
+  <si>
+    <t>2D08P</t>
+  </si>
+  <si>
+    <t>2D14P</t>
+  </si>
+  <si>
+    <t>2E07P</t>
+  </si>
+  <si>
+    <t>2F05P</t>
+  </si>
+  <si>
+    <t>2F18P</t>
+  </si>
+  <si>
+    <t>2G03P</t>
+  </si>
+  <si>
+    <t>3A22P</t>
+  </si>
+  <si>
+    <t>3A24P</t>
+  </si>
+  <si>
+    <t>3A25P</t>
+  </si>
+  <si>
+    <t>3B17P</t>
+  </si>
+  <si>
+    <t>3B23P</t>
+  </si>
+  <si>
+    <t>3C08P</t>
+  </si>
+  <si>
+    <t>4A02P</t>
+  </si>
+  <si>
+    <t>4A09P</t>
+  </si>
+  <si>
+    <t>4A27P</t>
+  </si>
+  <si>
+    <t>4A30P</t>
+  </si>
+  <si>
+    <t>4B15P</t>
+  </si>
+  <si>
+    <t>4B16P</t>
+  </si>
+  <si>
+    <t>4B17P</t>
+  </si>
+  <si>
+    <t>4B18P</t>
+  </si>
+  <si>
+    <t>4D11P</t>
   </si>
 </sst>
 </file>
@@ -10767,13 +11082,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1353"/>
+  <dimension ref="A1:K1403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1186" workbookViewId="0">
-      <selection activeCell="F1196" sqref="F1196"/>
+    <sheetView tabSelected="1" topLeftCell="A1374" workbookViewId="0">
+      <selection activeCell="C1375" sqref="C1375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -58124,7 +58442,1760 @@
         <v>180201000000</v>
       </c>
     </row>
+    <row r="1354" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1354" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1354" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1354" t="s">
+        <v>3347</v>
+      </c>
+      <c r="D1354" t="s">
+        <v>3397</v>
+      </c>
+      <c r="E1354" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1354">
+        <v>56.436859999999903</v>
+      </c>
+      <c r="G1354">
+        <v>-125.74169999999999</v>
+      </c>
+      <c r="H1354">
+        <v>3445</v>
+      </c>
+      <c r="I1354" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1354" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1354" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1355" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1355" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1355" t="s">
+        <v>3321</v>
+      </c>
+      <c r="D1355" t="s">
+        <v>3371</v>
+      </c>
+      <c r="E1355" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1355">
+        <v>52.595917</v>
+      </c>
+      <c r="G1355">
+        <v>-119.722694</v>
+      </c>
+      <c r="H1355">
+        <v>5381</v>
+      </c>
+      <c r="I1355" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1355" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1355" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1356" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1356" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1356" t="s">
+        <v>3306</v>
+      </c>
+      <c r="D1356" t="s">
+        <v>3355</v>
+      </c>
+      <c r="E1356" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1356">
+        <v>53.057337999999902</v>
+      </c>
+      <c r="G1356">
+        <v>-121.491828</v>
+      </c>
+      <c r="H1356">
+        <v>4823</v>
+      </c>
+      <c r="I1356" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1356" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1356" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1357" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1357" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1357" t="s">
+        <v>3327</v>
+      </c>
+      <c r="D1357" t="s">
+        <v>3377</v>
+      </c>
+      <c r="E1357" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1357">
+        <v>50.068552999999902</v>
+      </c>
+      <c r="G1357">
+        <v>-118.351122</v>
+      </c>
+      <c r="H1357">
+        <v>5315</v>
+      </c>
+      <c r="I1357" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1357" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1357" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1358" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1358" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1358" t="s">
+        <v>3337</v>
+      </c>
+      <c r="D1358" t="s">
+        <v>3387</v>
+      </c>
+      <c r="E1358" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1358">
+        <v>49.094139999999904</v>
+      </c>
+      <c r="G1358">
+        <v>-120.77249999999999</v>
+      </c>
+      <c r="H1358">
+        <v>6365</v>
+      </c>
+      <c r="I1358" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1358" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1358" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1359" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1359" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1359" t="s">
+        <v>3314</v>
+      </c>
+      <c r="D1359" t="s">
+        <v>3364</v>
+      </c>
+      <c r="E1359" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1359">
+        <v>52.106900000000003</v>
+      </c>
+      <c r="G1359">
+        <v>-120.867269999999</v>
+      </c>
+      <c r="H1359">
+        <v>4790</v>
+      </c>
+      <c r="I1359" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1359" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1359" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1360" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1360" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1360" t="s">
+        <v>3336</v>
+      </c>
+      <c r="D1360" t="s">
+        <v>3386</v>
+      </c>
+      <c r="E1360" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1360">
+        <v>49.862361</v>
+      </c>
+      <c r="G1360">
+        <v>-119.982111</v>
+      </c>
+      <c r="H1360">
+        <v>4790</v>
+      </c>
+      <c r="I1360" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1360" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1360" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1361" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1361" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1361" t="s">
+        <v>3343</v>
+      </c>
+      <c r="D1361" t="s">
+        <v>3393</v>
+      </c>
+      <c r="E1361" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1361">
+        <v>52.480888999999998</v>
+      </c>
+      <c r="G1361">
+        <v>-126.247833</v>
+      </c>
+      <c r="H1361">
+        <v>4364</v>
+      </c>
+      <c r="I1361" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1361" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1361" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1362" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1362" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1362" t="s">
+        <v>3351</v>
+      </c>
+      <c r="D1362" t="s">
+        <v>3401</v>
+      </c>
+      <c r="E1362" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1362">
+        <v>55.152027999999902</v>
+      </c>
+      <c r="G1362">
+        <v>-128.711028</v>
+      </c>
+      <c r="H1362">
+        <v>2904</v>
+      </c>
+      <c r="I1362" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1362" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1362" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1363" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1363" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1363" t="s">
+        <v>3324</v>
+      </c>
+      <c r="D1363" t="s">
+        <v>3374</v>
+      </c>
+      <c r="E1363" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1363">
+        <v>51.406664999999997</v>
+      </c>
+      <c r="G1363">
+        <v>-118.999725</v>
+      </c>
+      <c r="H1363">
+        <v>4921</v>
+      </c>
+      <c r="I1363" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1363" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1363" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1364" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1364" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1364" t="s">
+        <v>3318</v>
+      </c>
+      <c r="D1364" t="s">
+        <v>3368</v>
+      </c>
+      <c r="E1364" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1364">
+        <v>49.031500000000001</v>
+      </c>
+      <c r="G1364">
+        <v>-121.71210000000001</v>
+      </c>
+      <c r="H1364">
+        <v>5315</v>
+      </c>
+      <c r="I1364" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1364" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1364" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1365" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1365" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1365" t="s">
+        <v>3309</v>
+      </c>
+      <c r="D1365" t="s">
+        <v>3358</v>
+      </c>
+      <c r="E1365" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1365">
+        <v>53.626944999999999</v>
+      </c>
+      <c r="G1365">
+        <v>-121.016944</v>
+      </c>
+      <c r="H1365">
+        <v>5820</v>
+      </c>
+      <c r="I1365" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1365" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1365" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1366" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1366" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1366" t="s">
+        <v>3332</v>
+      </c>
+      <c r="D1366" t="s">
+        <v>3382</v>
+      </c>
+      <c r="E1366" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1366">
+        <v>50.639600000000002</v>
+      </c>
+      <c r="G1366">
+        <v>-116.929733</v>
+      </c>
+      <c r="H1366">
+        <v>6660</v>
+      </c>
+      <c r="I1366" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1366" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1366" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1367" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1367" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1367" t="s">
+        <v>3331</v>
+      </c>
+      <c r="D1367" t="s">
+        <v>3381</v>
+      </c>
+      <c r="E1367" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1367">
+        <v>51.059916999999999</v>
+      </c>
+      <c r="G1367">
+        <v>-116.137117</v>
+      </c>
+      <c r="H1367">
+        <v>6857</v>
+      </c>
+      <c r="I1367" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1367" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1367" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1368" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1368" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1368" t="s">
+        <v>3334</v>
+      </c>
+      <c r="D1368" t="s">
+        <v>3384</v>
+      </c>
+      <c r="E1368" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1368">
+        <v>49.551969999999997</v>
+      </c>
+      <c r="G1368">
+        <v>-118.6773</v>
+      </c>
+      <c r="H1368">
+        <v>6135</v>
+      </c>
+      <c r="I1368" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1368" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1368" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1369" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1369" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1369" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D1369" t="s">
+        <v>3362</v>
+      </c>
+      <c r="E1369" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1369">
+        <v>50.795632999999903</v>
+      </c>
+      <c r="G1369">
+        <v>-122.924542</v>
+      </c>
+      <c r="H1369">
+        <v>5840</v>
+      </c>
+      <c r="I1369" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1369" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1369" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1370" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1370" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1370" t="s">
+        <v>3307</v>
+      </c>
+      <c r="D1370" t="s">
+        <v>3356</v>
+      </c>
+      <c r="E1370" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1370">
+        <v>54.105719999999998</v>
+      </c>
+      <c r="G1370">
+        <v>-121</v>
+      </c>
+      <c r="H1370">
+        <v>3707</v>
+      </c>
+      <c r="I1370" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1370" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1370" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1371" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1371" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1371" t="s">
+        <v>3342</v>
+      </c>
+      <c r="D1371" t="s">
+        <v>3392</v>
+      </c>
+      <c r="E1371" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1371">
+        <v>48.969504999999998</v>
+      </c>
+      <c r="G1371">
+        <v>-124.27618200000001</v>
+      </c>
+      <c r="H1371">
+        <v>3806</v>
+      </c>
+      <c r="I1371" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1371" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1371" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1372" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1372" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1372" t="s">
+        <v>3352</v>
+      </c>
+      <c r="D1372" t="s">
+        <v>3402</v>
+      </c>
+      <c r="E1372" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1372">
+        <v>57.578689999999902</v>
+      </c>
+      <c r="G1372">
+        <v>-130.26273900000001</v>
+      </c>
+      <c r="H1372">
+        <v>3346</v>
+      </c>
+      <c r="I1372" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1372" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1372" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1373" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1373" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1373" t="s">
+        <v>3322</v>
+      </c>
+      <c r="D1373" t="s">
+        <v>3372</v>
+      </c>
+      <c r="E1373" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1373">
+        <v>52.203333999999998</v>
+      </c>
+      <c r="G1373">
+        <v>-120.016944</v>
+      </c>
+      <c r="H1373">
+        <v>5807</v>
+      </c>
+      <c r="I1373" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1373" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1373" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1374" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1374" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1374" t="s">
+        <v>3346</v>
+      </c>
+      <c r="D1374" t="s">
+        <v>3396</v>
+      </c>
+      <c r="E1374" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1374">
+        <v>57.623332999999903</v>
+      </c>
+      <c r="G1374">
+        <v>-125.073167</v>
+      </c>
+      <c r="H1374">
+        <v>5098</v>
+      </c>
+      <c r="I1374" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1374" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1374" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1375" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1375" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1375" t="s">
+        <v>3348</v>
+      </c>
+      <c r="D1375" t="s">
+        <v>3398</v>
+      </c>
+      <c r="E1375" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1375">
+        <v>54.196829999999999</v>
+      </c>
+      <c r="G1375">
+        <v>-126.30410000000001</v>
+      </c>
+      <c r="H1375">
+        <v>4265</v>
+      </c>
+      <c r="I1375" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1375" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1375" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1376" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1376" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1376" t="s">
+        <v>3305</v>
+      </c>
+      <c r="D1376" t="s">
+        <v>3354</v>
+      </c>
+      <c r="E1376" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1376">
+        <v>53.306039999999904</v>
+      </c>
+      <c r="G1376">
+        <v>-120.31926</v>
+      </c>
+      <c r="H1376">
+        <v>5282</v>
+      </c>
+      <c r="I1376" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1376" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1376" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1377" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1377" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1377" t="s">
+        <v>3335</v>
+      </c>
+      <c r="D1377" t="s">
+        <v>3385</v>
+      </c>
+      <c r="E1377" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1377">
+        <v>49.944669999999903</v>
+      </c>
+      <c r="G1377">
+        <v>-118.94970000000001</v>
+      </c>
+      <c r="H1377">
+        <v>5840</v>
+      </c>
+      <c r="I1377" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1377" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1377" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1378" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1378" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1378" t="s">
+        <v>3313</v>
+      </c>
+      <c r="D1378" t="s">
+        <v>3363</v>
+      </c>
+      <c r="E1378" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1378">
+        <v>50.762555999999996</v>
+      </c>
+      <c r="G1378">
+        <v>-122.207694</v>
+      </c>
+      <c r="H1378">
+        <v>6070</v>
+      </c>
+      <c r="I1378" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1378" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1378" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1379" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1379" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1379" t="s">
+        <v>3326</v>
+      </c>
+      <c r="D1379" t="s">
+        <v>3376</v>
+      </c>
+      <c r="E1379" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1379">
+        <v>52.220555999999902</v>
+      </c>
+      <c r="G1379">
+        <v>-118.22583299999999</v>
+      </c>
+      <c r="H1379">
+        <v>6348</v>
+      </c>
+      <c r="I1379" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1379" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1379" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1380" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1380" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1380" t="s">
+        <v>3329</v>
+      </c>
+      <c r="D1380" t="s">
+        <v>3379</v>
+      </c>
+      <c r="E1380" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1380">
+        <v>49.447221999999996</v>
+      </c>
+      <c r="G1380">
+        <v>-114.97499999999999</v>
+      </c>
+      <c r="H1380">
+        <v>6102</v>
+      </c>
+      <c r="I1380" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1380" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1380" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1381" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1381" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1381" t="s">
+        <v>3339</v>
+      </c>
+      <c r="D1381" t="s">
+        <v>3389</v>
+      </c>
+      <c r="E1381" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1381">
+        <v>51.77617</v>
+      </c>
+      <c r="G1381">
+        <v>-124.62179999999999</v>
+      </c>
+      <c r="H1381">
+        <v>5413</v>
+      </c>
+      <c r="I1381" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1381" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1381" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1382" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1382" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1382" t="s">
+        <v>3320</v>
+      </c>
+      <c r="D1382" t="s">
+        <v>3370</v>
+      </c>
+      <c r="E1382" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1382">
+        <v>52.182139999999997</v>
+      </c>
+      <c r="G1382">
+        <v>-119.3227</v>
+      </c>
+      <c r="H1382">
+        <v>5151</v>
+      </c>
+      <c r="I1382" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1382" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1382" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1383" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1383" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1383" t="s">
+        <v>3325</v>
+      </c>
+      <c r="D1383" t="s">
+        <v>3375</v>
+      </c>
+      <c r="E1383" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1383">
+        <v>51.036341999999998</v>
+      </c>
+      <c r="G1383">
+        <v>-118.15160299999999</v>
+      </c>
+      <c r="H1383">
+        <v>6070</v>
+      </c>
+      <c r="I1383" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1383" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1383" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1384" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1384" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1384" t="s">
+        <v>3310</v>
+      </c>
+      <c r="D1384" t="s">
+        <v>3359</v>
+      </c>
+      <c r="E1384" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1384">
+        <v>53.728609999999897</v>
+      </c>
+      <c r="G1384">
+        <v>-126.423614</v>
+      </c>
+      <c r="H1384">
+        <v>4888</v>
+      </c>
+      <c r="I1384" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1384" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1384" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1385" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1385" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1385" t="s">
+        <v>3330</v>
+      </c>
+      <c r="D1385" t="s">
+        <v>3380</v>
+      </c>
+      <c r="E1385" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1385">
+        <v>49.2515</v>
+      </c>
+      <c r="G1385">
+        <v>-115.7739</v>
+      </c>
+      <c r="H1385">
+        <v>6020</v>
+      </c>
+      <c r="I1385" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1385" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1385" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1386" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1386" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1386" t="s">
+        <v>3312</v>
+      </c>
+      <c r="D1386" t="s">
+        <v>3361</v>
+      </c>
+      <c r="E1386" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1386">
+        <v>53.152500000000003</v>
+      </c>
+      <c r="G1386">
+        <v>-126.881111</v>
+      </c>
+      <c r="H1386">
+        <v>4593</v>
+      </c>
+      <c r="I1386" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1386" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1386" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1387" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1387" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1387" t="s">
+        <v>3338</v>
+      </c>
+      <c r="D1387" t="s">
+        <v>3388</v>
+      </c>
+      <c r="E1387" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1387">
+        <v>51.243249999999897</v>
+      </c>
+      <c r="G1387">
+        <v>-124.45958299999999</v>
+      </c>
+      <c r="H1387">
+        <v>4921</v>
+      </c>
+      <c r="I1387" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1387" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1387" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1388" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1388" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1388" t="s">
+        <v>3323</v>
+      </c>
+      <c r="D1388" t="s">
+        <v>3373</v>
+      </c>
+      <c r="E1388" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1388">
+        <v>50.44961</v>
+      </c>
+      <c r="G1388">
+        <v>-118.61856</v>
+      </c>
+      <c r="H1388">
+        <v>6201</v>
+      </c>
+      <c r="I1388" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1388" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1388" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1389" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1389" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1389" t="s">
+        <v>3344</v>
+      </c>
+      <c r="D1389" t="s">
+        <v>3394</v>
+      </c>
+      <c r="E1389" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1389">
+        <v>55.353000000000002</v>
+      </c>
+      <c r="G1389">
+        <v>-122.637333</v>
+      </c>
+      <c r="H1389">
+        <v>4593</v>
+      </c>
+      <c r="I1389" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1389" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1389" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1390" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1390" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1390" t="s">
+        <v>3345</v>
+      </c>
+      <c r="D1390" t="s">
+        <v>3395</v>
+      </c>
+      <c r="E1390" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1390">
+        <v>57.548583000000001</v>
+      </c>
+      <c r="G1390">
+        <v>-126.74831399999999</v>
+      </c>
+      <c r="H1390">
+        <v>4301</v>
+      </c>
+      <c r="I1390" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1390" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1390" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1391" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1391" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1391" t="s">
+        <v>3333</v>
+      </c>
+      <c r="D1391" t="s">
+        <v>3383</v>
+      </c>
+      <c r="E1391" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1391">
+        <v>49.690079999999902</v>
+      </c>
+      <c r="G1391">
+        <v>-117.0865</v>
+      </c>
+      <c r="H1391">
+        <v>6890</v>
+      </c>
+      <c r="I1391" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1391" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1391" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1392" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1392" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1392" t="s">
+        <v>3308</v>
+      </c>
+      <c r="D1392" t="s">
+        <v>3357</v>
+      </c>
+      <c r="E1392" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1392">
+        <v>53.784219999999998</v>
+      </c>
+      <c r="G1392">
+        <v>-120.37520000000001</v>
+      </c>
+      <c r="H1392">
+        <v>5512</v>
+      </c>
+      <c r="I1392" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1392" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1392" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1393" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1393" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1393" t="s">
+        <v>3349</v>
+      </c>
+      <c r="D1393" t="s">
+        <v>3399</v>
+      </c>
+      <c r="E1393" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1393">
+        <v>55.861652999999997</v>
+      </c>
+      <c r="G1393">
+        <v>-127.69842</v>
+      </c>
+      <c r="H1393">
+        <v>4856</v>
+      </c>
+      <c r="I1393" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1393" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1393" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1394" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1394" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1394" t="s">
+        <v>3319</v>
+      </c>
+      <c r="D1394" t="s">
+        <v>3369</v>
+      </c>
+      <c r="E1394" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1394">
+        <v>49.660830999999902</v>
+      </c>
+      <c r="G1394">
+        <v>-121.660834999999</v>
+      </c>
+      <c r="H1394">
+        <v>3871</v>
+      </c>
+      <c r="I1394" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1394" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1394" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1395" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1395" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1395" t="s">
+        <v>3340</v>
+      </c>
+      <c r="D1395" t="s">
+        <v>3390</v>
+      </c>
+      <c r="E1395" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1395">
+        <v>50.154299999999999</v>
+      </c>
+      <c r="G1395">
+        <v>-123.4361</v>
+      </c>
+      <c r="H1395">
+        <v>4462</v>
+      </c>
+      <c r="I1395" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1395" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1395" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1396" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1396" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1396" t="s">
+        <v>3328</v>
+      </c>
+      <c r="D1396" t="s">
+        <v>3378</v>
+      </c>
+      <c r="E1396" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1396">
+        <v>50.434171999999997</v>
+      </c>
+      <c r="G1396">
+        <v>-117.70121399999999</v>
+      </c>
+      <c r="H1396">
+        <v>5906</v>
+      </c>
+      <c r="I1396" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1396" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1396" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1397" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1397" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1397" t="s">
+        <v>3311</v>
+      </c>
+      <c r="D1397" t="s">
+        <v>3360</v>
+      </c>
+      <c r="E1397" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1397">
+        <v>53.593055</v>
+      </c>
+      <c r="G1397">
+        <v>-127.64389</v>
+      </c>
+      <c r="H1397">
+        <v>4265</v>
+      </c>
+      <c r="I1397" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1397" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1397" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1398" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1398" t="s">
+        <v>3316</v>
+      </c>
+      <c r="D1398" t="s">
+        <v>3366</v>
+      </c>
+      <c r="E1398" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1398">
+        <v>50.536249999999903</v>
+      </c>
+      <c r="G1398">
+        <v>-122.92995999999999</v>
+      </c>
+      <c r="H1398">
+        <v>5512</v>
+      </c>
+      <c r="I1398" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1398" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1398" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1399" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1399" t="s">
+        <v>3350</v>
+      </c>
+      <c r="D1399" t="s">
+        <v>3400</v>
+      </c>
+      <c r="E1399" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1399">
+        <v>54.645905999999997</v>
+      </c>
+      <c r="G1399">
+        <v>-127.674272</v>
+      </c>
+      <c r="H1399">
+        <v>4462</v>
+      </c>
+      <c r="I1399" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1399" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1399" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1400" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1400" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1400" t="s">
+        <v>3317</v>
+      </c>
+      <c r="D1400" t="s">
+        <v>3367</v>
+      </c>
+      <c r="E1400" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1400">
+        <v>49.232749999999903</v>
+      </c>
+      <c r="G1400">
+        <v>-121.579883</v>
+      </c>
+      <c r="H1400">
+        <v>4856</v>
+      </c>
+      <c r="I1400" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1400" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1400" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1401" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1401" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1401" t="s">
+        <v>3341</v>
+      </c>
+      <c r="D1401" t="s">
+        <v>3391</v>
+      </c>
+      <c r="E1401" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1401">
+        <v>49.704138999999998</v>
+      </c>
+      <c r="G1401">
+        <v>-125.67925</v>
+      </c>
+      <c r="H1401">
+        <v>4888</v>
+      </c>
+      <c r="I1401" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1401" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1401" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1402" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1402" t="s">
+        <v>3315</v>
+      </c>
+      <c r="D1402" t="s">
+        <v>3365</v>
+      </c>
+      <c r="E1402" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1402">
+        <v>52.832009999999997</v>
+      </c>
+      <c r="G1402">
+        <v>-121.35563999999999</v>
+      </c>
+      <c r="H1402">
+        <v>5479</v>
+      </c>
+      <c r="I1402" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1402" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1402" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1403" t="s">
+        <v>2556</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1403" t="s">
+        <v>3304</v>
+      </c>
+      <c r="D1403" t="s">
+        <v>3353</v>
+      </c>
+      <c r="E1403" t="s">
+        <v>3302</v>
+      </c>
+      <c r="F1403">
+        <v>52.906219999999998</v>
+      </c>
+      <c r="G1403">
+        <v>-118.5475</v>
+      </c>
+      <c r="H1403">
+        <v>6102</v>
+      </c>
+      <c r="I1403" t="s">
+        <v>3302</v>
+      </c>
+      <c r="J1403" t="s">
+        <v>3302</v>
+      </c>
+      <c r="K1403" t="s">
+        <v>3302</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1354:I1403">
+    <sortCondition ref="C1354:C1403"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>